<commit_message>
Before Fixing the last instruction in 2 operands
</commit_message>
<xml_diff>
--- a/Integration/Testing Integration.xlsx
+++ b/Integration/Testing Integration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496315A5-AD27-4A12-8E91-237960DC5705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48738C0-55BE-4805-8F2C-E8C033205FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25335" yWindow="375" windowWidth="25470" windowHeight="15420" xr2:uid="{84B84772-55DC-4D49-8B71-DEE464C5FD95}"/>
+    <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{84B84772-55DC-4D49-8B71-DEE464C5FD95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -647,9 +647,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -698,6 +695,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DB27A1-D3B1-4D9C-B8AF-56FD1DC15792}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,13 +1026,13 @@
     <col min="2" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
     <col min="8" max="8" width="20.5546875" customWidth="1"/>
     <col min="9" max="9" width="17.21875" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" customWidth="1"/>
     <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="19.21875" customWidth="1"/>
     <col min="13" max="13" width="18.88671875" customWidth="1"/>
     <col min="14" max="14" width="23.44140625" customWidth="1"/>
     <col min="15" max="15" width="19.44140625" customWidth="1"/>
@@ -1043,62 +1043,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>3</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>5</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>6</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>7</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>8</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="6">
-        <v>10</v>
-      </c>
-      <c r="L2" s="5">
+      <c r="K2" s="5">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4">
         <v>11</v>
       </c>
-      <c r="M2" s="6">
-        <v>12</v>
-      </c>
-      <c r="N2" s="5">
-        <v>13</v>
-      </c>
-      <c r="O2" s="6">
-        <v>14</v>
-      </c>
-      <c r="P2" s="5">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="6">
+      <c r="M2" s="5">
+        <v>12</v>
+      </c>
+      <c r="N2" s="4">
+        <v>13</v>
+      </c>
+      <c r="O2" s="5">
+        <v>14</v>
+      </c>
+      <c r="P2" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="5">
         <v>16</v>
       </c>
     </row>
@@ -1106,362 +1106,362 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="B3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="9"/>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="9"/>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="8"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="9"/>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="8"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="9"/>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="8"/>
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q13" s="13" t="s">
+      <c r="B13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1516,508 +1516,508 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>2</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>3</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>4</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>5</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>6</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>7</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <v>8</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <v>9</v>
       </c>
-      <c r="K21" s="4">
-        <v>10</v>
-      </c>
-      <c r="L21" s="4">
+      <c r="K21" s="3">
+        <v>10</v>
+      </c>
+      <c r="L21" s="3">
         <v>11</v>
       </c>
-      <c r="M21" s="4">
-        <v>12</v>
-      </c>
-      <c r="N21" s="4">
-        <v>13</v>
-      </c>
-      <c r="O21" s="4">
-        <v>14</v>
-      </c>
-      <c r="P21" s="4">
-        <v>15</v>
-      </c>
-      <c r="Q21" s="4">
-        <v>16</v>
-      </c>
-      <c r="R21" s="4">
+      <c r="M21" s="3">
+        <v>12</v>
+      </c>
+      <c r="N21" s="3">
+        <v>13</v>
+      </c>
+      <c r="O21" s="3">
+        <v>14</v>
+      </c>
+      <c r="P21" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>16</v>
+      </c>
+      <c r="R21" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="22"/>
+      <c r="B22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="21"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="23"/>
+      <c r="B23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="22"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="23"/>
+      <c r="B24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="22"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="23"/>
+      <c r="B25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="22"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="23"/>
+      <c r="B26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="22"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="L27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="23"/>
+      <c r="B27" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="22"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="M28" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="23"/>
+      <c r="B28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="22"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="M29" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="N29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="23"/>
+      <c r="B29" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="22"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L30" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="M30" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="O30" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="23"/>
+      <c r="B30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="22"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M31" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="N31" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="O31" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="P31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="23"/>
+      <c r="B31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="22"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P32" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="R32" s="23"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R32" s="22"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N33" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="O33" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="P33" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q33" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="R33" s="25" t="s">
+      <c r="B33" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="P33" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="R33" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O34" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P34" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q34" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="R34" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="S34" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B34" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R34" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="S34" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="175.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Before fixing sw interrupt
</commit_message>
<xml_diff>
--- a/Integration/Testing Integration.xlsx
+++ b/Integration/Testing Integration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48738C0-55BE-4805-8F2C-E8C033205FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F172BB45-8BC5-4E22-A485-9FAB8D734469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{84B84772-55DC-4D49-8B71-DEE464C5FD95}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
   <si>
     <t>HLT</t>
   </si>
@@ -503,18 +503,280 @@
 OutPort: XXXX
 InPort: XXXX</t>
   </si>
+  <si>
+    <t>TESTING BRANCHING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN R1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN R2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN R3  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN R4  </t>
+  </si>
+  <si>
+    <t>Push R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT 1  </t>
+  </si>
+  <si>
+    <t>AND R5,R1,R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT R5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT 0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN  R6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JN  700 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SETC </t>
+  </si>
+  <si>
+    <t>INC R6</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP R6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call 300 </t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <r>
+      <t>INC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>R1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(NOT EXECUTED)</t>
+    </r>
+  </si>
+  <si>
+    <t>INC R1  (NOT EXECUTED)</t>
+  </si>
+  <si>
+    <t>SETC   (NOT EXECUTED)</t>
+  </si>
+  <si>
+    <t>JMP 30  (TAKEN)</t>
+  </si>
+  <si>
+    <t>JZ  50  (TAKEN)</t>
+  </si>
+  <si>
+    <t>JZ 30  (NOT TAKEN)</t>
+  </si>
+  <si>
+    <t>JC 100  (NOT TAKEN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD R6,R3,R6 </t>
+  </si>
+  <si>
+    <t>ADD R1,R1,R2</t>
+  </si>
+  <si>
+    <t>AND R0,R0,R0</t>
+  </si>
+  <si>
+    <t>RTI</t>
+  </si>
+  <si>
+    <t>SETC (HW)</t>
+  </si>
+  <si>
+    <t>AND R0,R0,R0 (HW)</t>
+  </si>
+  <si>
+    <t>OUT R3 ((HW)</t>
+  </si>
+  <si>
+    <t>RTI (HW)</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 0
+R2: 0
+R3: 0
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: XXXX
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 0
+R2: 0
+R3: 0
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: 00000030
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 0
+R2: 0
+R3: 0
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: 00000050
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 0
+R2: 0
+R3: 0
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: 00000100
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AND R0,R0,R0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTI  </t>
+  </si>
+  <si>
+    <t>OUT R6</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 00000030
+R2: 0
+R3: 0
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: 00000300
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 00000030
+R2: 00000050
+R3: 0
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: XXXXX
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 00000030
+R2: 00000050
+R3: 00000100
+R4: 0
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: XXXXX
+SP: 000FFFFF</t>
+  </si>
+  <si>
+    <t>R0: 0
+R1: 00000030
+R2: 00000050
+R3: 00000100
+R4: 00000300
+R5: 0
+R6: 0
+R7: 0
+PC_Concat: 000
+OutPort: XXXX
+InPort: XXXXX
+SP: 000FFFFF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -641,7 +903,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -700,6 +962,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,15 +1277,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DB27A1-D3B1-4D9C-B8AF-56FD1DC15792}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K39" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
     <col min="2" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="21.109375" customWidth="1"/>
@@ -2073,10 +2336,1103 @@
         <v>58</v>
       </c>
     </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H40" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3">
+        <v>4</v>
+      </c>
+      <c r="F41" s="3">
+        <v>5</v>
+      </c>
+      <c r="G41" s="3">
+        <v>6</v>
+      </c>
+      <c r="H41" s="3">
+        <v>7</v>
+      </c>
+      <c r="I41" s="3">
+        <v>8</v>
+      </c>
+      <c r="J41" s="3">
+        <v>9</v>
+      </c>
+      <c r="K41" s="3">
+        <v>10</v>
+      </c>
+      <c r="L41" s="3">
+        <v>11</v>
+      </c>
+      <c r="M41" s="3">
+        <v>12</v>
+      </c>
+      <c r="N41" s="3">
+        <v>13</v>
+      </c>
+      <c r="O41" s="3">
+        <v>14</v>
+      </c>
+      <c r="P41" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>16</v>
+      </c>
+      <c r="R41" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L47" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M48" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="13"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13"/>
+      <c r="S54" s="13"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
+      <c r="S56" s="13"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
+      <c r="S58" s="13"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="13"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+      <c r="S60" s="13"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+      <c r="S61" s="13"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+      <c r="S62" s="13"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
+      <c r="S63" s="13"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+      <c r="S64" s="13"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="13"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="13"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A67" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="13"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="13"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="13"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="13"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A71" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A72" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="13"/>
+      <c r="N72" s="13"/>
+      <c r="O72" s="13"/>
+      <c r="P72" s="13"/>
+      <c r="Q72" s="13"/>
+      <c r="R72" s="13"/>
+      <c r="S72" s="13"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A73" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="13"/>
+      <c r="R73" s="13"/>
+      <c r="S73" s="13"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A74" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13"/>
+      <c r="O74" s="13"/>
+      <c r="P74" s="13"/>
+      <c r="Q74" s="13"/>
+      <c r="R74" s="13"/>
+      <c r="S74" s="13"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A75" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="13"/>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="13"/>
+      <c r="R75" s="13"/>
+      <c r="S75" s="13"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A76" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
+      <c r="O76" s="13"/>
+      <c r="P76" s="13"/>
+      <c r="Q76" s="13"/>
+      <c r="R76" s="13"/>
+      <c r="S76" s="13"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
+      <c r="O77" s="13"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A78" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
+      <c r="O78" s="13"/>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="13"/>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13"/>
+      <c r="O79" s="13"/>
+      <c r="P79" s="13"/>
+      <c r="Q79" s="13"/>
+      <c r="R79" s="13"/>
+      <c r="S79" s="13"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A80" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="13"/>
+      <c r="N80" s="13"/>
+      <c r="O80" s="13"/>
+      <c r="P80" s="13"/>
+      <c r="Q80" s="13"/>
+      <c r="R80" s="13"/>
+      <c r="S80" s="13"/>
+    </row>
+    <row r="81" spans="2:19" ht="227.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R81" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S81" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="G20:L20"/>
+    <mergeCell ref="H40:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>